<commit_message>
mise en place du code de la base de données
</commit_message>
<xml_diff>
--- a/methode_agiles/Burndown_Chart_Projet.xlsx
+++ b/methode_agiles/Burndown_Chart_Projet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p2101440\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projet\Projet\methode_agiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B45F40-19CB-47C3-A88A-69F82ABB0B27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D84C90-28EF-495A-8E7D-9EDF1A7A8696}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Burndown_Chart</a:t>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1506,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>